<commit_message>
feat: Updated JavaScript, HTML, and Excel Reference File
- Refactored JavaScript code for better readability.
- Added comments for code sections.
- Fixed a typo in a function name.
- Improved handling of removal unit button.
- Added a test scenario for unit change.
- Updated HTML to match JavaScript changes.
- Fixed a typo in the HTML button element.
- Updated the Excel reference file: Pipeline Price CheatSheet.xlsx.
</commit_message>
<xml_diff>
--- a/Pipeline Price CheatSheet.xlsx
+++ b/Pipeline Price CheatSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abalkaran\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayb\Desktop\CODE\pipelineCheatsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588E1855-D614-4BCA-8C14-53DE435AD513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BA5817-87BA-4302-AA83-0AA399943CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41820" yWindow="2880" windowWidth="27945" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4116" yWindow="1500" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DISCOUNT" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -235,13 +234,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.000%"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="_-&quot;$&quot;* #,##0.000_-;\-&quot;$&quot;* #,##0.000_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="173" formatCode="_([$$-409]* #,##0.000_);_([$$-409]* \(#,##0.000\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -556,7 +557,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -688,6 +689,33 @@
     <xf numFmtId="9" fontId="4" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="12" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -700,37 +728,15 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="12" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="173" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1045,36 +1051,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="1" customWidth="1"/>
-    <col min="2" max="7" width="20.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" style="1" customWidth="1"/>
-    <col min="9" max="25" width="20.7109375" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="27.109375" style="1" customWidth="1"/>
+    <col min="2" max="7" width="20.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" style="1" customWidth="1"/>
+    <col min="9" max="25" width="20.6640625" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
       <c r="G1" s="45"/>
     </row>
-    <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="44"/>
       <c r="E2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1093,7 @@
       <c r="E3" s="15">
         <v>1550.25</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="66">
         <f>E3*0.1</f>
         <v>155.02500000000001</v>
       </c>
@@ -1100,56 +1106,56 @@
         <v>1395.2250000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E4" s="43"/>
       <c r="F4" s="43"/>
       <c r="G4" s="43"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F5" s="43"/>
       <c r="G5" s="43"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="53" t="s">
+    <row r="7" spans="1:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="63"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="67">
         <f>E3-B9</f>
-        <v>1545.25</v>
-      </c>
-      <c r="F8" s="57">
-        <f>0/B3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1395.2249999999999</v>
+      </c>
+      <c r="F8" s="68">
+        <f>(E8/B3)</f>
+        <v>0.37245728777362519</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="16">
-        <v>5</v>
+        <v>155.02500000000001</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1158,10 +1164,14 @@
       </c>
       <c r="E10" s="12">
         <f>1-(E8/B3)</f>
-        <v>0.58749332621462891</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.62754271222637481</v>
+      </c>
+      <c r="F10" s="49">
+        <f>1-(E3/B3)</f>
+        <v>0.58615856914041642</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1170,49 +1180,49 @@
       <c r="F11" s="44"/>
       <c r="G11" s="46"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G12" s="1">
         <f>(DISCOUNT!B18/DISCOUNT!B16)</f>
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G13" s="43"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H14" s="43"/>
     </row>
-    <row r="15" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="53" t="s">
+    <row r="15" spans="1:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="54"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="63"/>
       <c r="K15" s="1">
         <f>55/100</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="58">
+      <c r="B16" s="53">
         <v>0.55000000000000004</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="61">
+      <c r="E16" s="56">
         <f>E3*(1-B20)</f>
         <v>1395.2250000000001</v>
       </c>
       <c r="G16" s="49"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1231,18 +1241,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="59">
+      <c r="B18" s="54">
         <v>570.35</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="58">
+      <c r="E18" s="53">
         <v>0.6</v>
       </c>
       <c r="G18" s="1">
@@ -1253,7 +1263,7 @@
         <f>G18/(1-DISCOUNT!E18)</f>
         <v>2708.9999999999995</v>
       </c>
-      <c r="I18" s="65">
+      <c r="I18" s="57">
         <f>G18-(DISCOUNT!$E$3*DISCOUNT!B20)</f>
         <v>928.57499999999993</v>
       </c>
@@ -1262,39 +1272,39 @@
         <v>0.65722591362126237</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="62" t="s">
+      <c r="F19" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="62"/>
-      <c r="H19" s="67" t="s">
+      <c r="G19" s="61"/>
+      <c r="H19" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="63" t="s">
+      <c r="I19" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="J19" s="63"/>
+      <c r="J19" s="60"/>
       <c r="K19" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="60">
+      <c r="B20" s="55">
         <v>0.1</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="66">
+      <c r="E20" s="58">
         <f>1-(Sheet2!L4/Sheet2!K4)</f>
         <v>0.65722591362126237</v>
       </c>
@@ -1310,7 +1320,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1320,25 +1330,25 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F23" s="49"/>
       <c r="H23" s="43"/>
     </row>
-    <row r="25" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="53" t="s">
+    <row r="25" spans="1:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="64" t="s">
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="G25" s="63"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="60"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1346,7 +1356,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>6</v>
       </c>
@@ -1362,43 +1372,43 @@
         <v>0.63581954084356651</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H31" s="43"/>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="53" t="s">
+    <row r="35" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="54"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="62"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="63"/>
+    </row>
+    <row r="36" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1413,7 +1423,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>9</v>
       </c>
@@ -1424,7 +1434,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1439,7 +1449,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1449,6 +1459,7 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="8">
+    <mergeCell ref="A35:E35"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="F19:G19"/>
@@ -1456,7 +1467,6 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A35:E35"/>
   </mergeCells>
   <conditionalFormatting sqref="H18">
     <cfRule type="expression" dxfId="3" priority="1">
@@ -1500,40 +1510,40 @@
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="H1" s="56" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="H1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="O1" s="56" t="s">
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="O1" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-    </row>
-    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+    </row>
+    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20"/>
       <c r="B2" s="40" t="s">
         <v>30</v>
@@ -1571,7 +1581,7 @@
       </c>
       <c r="T2" s="20"/>
     </row>
-    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20"/>
       <c r="B3" s="39" t="s">
         <v>29</v>
@@ -1612,7 +1622,7 @@
       </c>
       <c r="T3" s="20"/>
     </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20"/>
       <c r="B4" s="38" t="s">
         <v>28</v>
@@ -1653,7 +1663,7 @@
       </c>
       <c r="T4" s="20"/>
     </row>
-    <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20"/>
       <c r="B5" s="38" t="s">
         <v>27</v>
@@ -1694,7 +1704,7 @@
       </c>
       <c r="T5" s="20"/>
     </row>
-    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20"/>
       <c r="B6" s="38" t="s">
         <v>26</v>
@@ -1735,7 +1745,7 @@
       </c>
       <c r="T6" s="20"/>
     </row>
-    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20"/>
       <c r="B7" s="38" t="s">
         <v>25</v>
@@ -1776,7 +1786,7 @@
       </c>
       <c r="T7" s="20"/>
     </row>
-    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="20"/>
       <c r="B8" s="38" t="s">
         <v>24</v>
@@ -1817,7 +1827,7 @@
       </c>
       <c r="T8" s="20"/>
     </row>
-    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20"/>
       <c r="B9" s="38" t="s">
         <v>23</v>
@@ -1858,7 +1868,7 @@
       </c>
       <c r="T9" s="20"/>
     </row>
-    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="20"/>
       <c r="B10" s="37" t="s">
         <v>22</v>
@@ -1899,7 +1909,7 @@
       </c>
       <c r="T10" s="20"/>
     </row>
-    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="20"/>
       <c r="B11" s="35" t="s">
         <v>21</v>
@@ -1937,7 +1947,7 @@
       </c>
       <c r="T11" s="20"/>
     </row>
-    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="20"/>
       <c r="B12" s="31" t="s">
         <v>18</v>
@@ -1978,7 +1988,7 @@
       </c>
       <c r="T12" s="20"/>
     </row>
-    <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="20"/>
       <c r="B13" s="29" t="s">
         <v>17</v>
@@ -2019,7 +2029,7 @@
       </c>
       <c r="T13" s="20"/>
     </row>
-    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20"/>
       <c r="B14" s="29" t="s">
         <v>16</v>
@@ -2060,7 +2070,7 @@
       </c>
       <c r="T14" s="20"/>
     </row>
-    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="20"/>
       <c r="B15" s="29" t="s">
         <v>15</v>
@@ -2101,7 +2111,7 @@
       </c>
       <c r="T15" s="20"/>
     </row>
-    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20"/>
       <c r="B16" s="29" t="s">
         <v>14</v>
@@ -2142,7 +2152,7 @@
       </c>
       <c r="T16" s="20"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
       <c r="B17" s="28" t="s">
         <v>13</v>
@@ -2183,7 +2193,7 @@
       </c>
       <c r="T17" s="20"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
       <c r="C18" s="24"/>
@@ -2203,7 +2213,7 @@
       <c r="S18" s="20"/>
       <c r="T18" s="20"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
       <c r="C19" s="23"/>
@@ -2256,30 +2266,30 @@
       <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="11" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" customWidth="1"/>
+    <col min="11" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:12" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
-      <c r="H2" s="53" t="s">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
+      <c r="H2" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="54"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="63"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>DISCOUNT!B27</f>
         <v>0.12</v>
@@ -2294,7 +2304,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>DISCOUNT!E3*A3</f>
         <v>186.03</v>
@@ -2312,14 +2322,14 @@
         <v>928.57499999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
+    <row r="6" spans="1:12" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="54"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="63"/>
       <c r="H6" t="s">
         <v>43</v>
       </c>
@@ -2330,7 +2340,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <f>1-DISCOUNT!B37</f>
         <v>0.75</v>
@@ -2345,7 +2355,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H8" s="50">
         <v>0.55000000000000004</v>
       </c>
@@ -2356,11 +2366,11 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H9" s="51"/>
       <c r="K9" s="51"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H10" s="51"/>
       <c r="K10" s="51"/>
     </row>

</xml_diff>